<commit_message>
'SET' message, added R modes, disabled unused parameters, fixed bugs
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="13986" windowWidth="25786" xWindow="-93" yWindow="-93"/>
+    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="13720" windowWidth="25313" xWindow="80" yWindow="80"/>
   </bookViews>
   <sheets>
     <sheet name="USERS" sheetId="1" state="visible" r:id="rId1"/>
@@ -352,7 +352,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.35" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.35"/>
   <cols>
     <col customWidth="1" max="1" min="1" style="1" width="15"/>
     <col customWidth="1" max="2" min="2" style="1" width="10.87890625"/>
@@ -383,12 +383,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>hello</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>hello</t>
         </is>
       </c>
     </row>
@@ -413,11 +413,31 @@
         <f>ROW()</f>
         <v/>
       </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5">
         <f>ROW()</f>
         <v/>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -480,7 +500,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="20.3515625" defaultRowHeight="14.35" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="20.3515625" defaultRowHeight="14.35"/>
   <cols>
     <col customWidth="1" max="5" min="5" style="1" width="25.234375"/>
     <col customWidth="1" max="6" min="6" style="1" width="21.41015625"/>
@@ -574,17 +594,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>DOO</t>
+          <t>AOO</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>50</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>50</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -594,17 +614,17 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
           <t>3.5</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>3.5</t>
-        </is>
-      </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>0.4</t>
+          <t>0.05</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -614,27 +634,27 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>320</t>
+          <t>500</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>250</t>
+          <t>500</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Med</t>
+          <t>V-Low</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>50</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>5</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -650,7 +670,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>DOO</t>
+          <t>AAI</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -670,7 +690,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>3.5</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -724,6 +744,11 @@
         <f>ROW()</f>
         <v/>
       </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>AOO</t>
+        </is>
+      </c>
       <c r="C4" t="inlineStr">
         <is>
           <t>60</t>
@@ -794,6 +819,76 @@
       <c r="A5">
         <f>ROW()</f>
         <v/>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>AOO</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>3.5</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>3.5</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>0.4</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>0.5</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>320</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>250</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>Med</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
     </row>
     <row r="6">

</xml_diff>

<commit_message>
serial comm added to set all button
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -352,7 +352,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.35"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.35" outlineLevelCol="0"/>
   <cols>
     <col customWidth="1" max="1" min="1" style="1" width="15"/>
     <col customWidth="1" max="2" min="2" style="1" width="10.87890625"/>
@@ -500,7 +500,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="20.3515625" defaultRowHeight="14.35"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="20.3515625" defaultRowHeight="14.35" outlineLevelCol="0"/>
   <cols>
     <col customWidth="1" max="5" min="5" style="1" width="25.234375"/>
     <col customWidth="1" max="6" min="6" style="1" width="21.41015625"/>
@@ -594,17 +594,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>AOO</t>
+          <t>VVI</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>40</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>120</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -614,7 +614,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>3.5</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -624,7 +624,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>0.05</t>
+          <t>0.4</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -634,27 +634,27 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>500</t>
+          <t>320</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>500</t>
+          <t>250</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>V-Low</t>
+          <t>Med</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>30</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>8</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">

</xml_diff>